<commit_message>
report update and data tuning
</commit_message>
<xml_diff>
--- a/report/references.xlsx
+++ b/report/references.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\year3\IN3007-IndividualProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\year3\IN3007-IndividualProject\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB2C257-E3CA-48FB-9529-82D8333EFC69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E2D8E8-D701-4D76-B2F2-794695BC6004}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1575" yWindow="2715" windowWidth="27225" windowHeight="11385" xr2:uid="{64E3EF4A-D857-422D-A798-7481F9C38A08}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64E3EF4A-D857-422D-A798-7481F9C38A08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>reference</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>Coifman, B., Beymer, D., McLauchlan, P., &amp; Malik, J. (1998). A real-time computer vision system for vehicle tracking and traffic surveillance. Transportation Research Part C: Emerging Technologies</t>
-  </si>
-  <si>
-    <t>(Coifman, 1998)</t>
   </si>
   <si>
     <t>SZELISKI, R., 2020. COMPUTER VISION. SPRINGER NATURE, p.5.</t>
@@ -85,38 +82,74 @@
     <t xml:space="preserve">Chavdarova, T., Baqué, P., Bouquet, S., Maksai, A., Jose, C., Lettry, L., Fua, P., Van Gool, L. and Fleuret, F., 2017. The wildtrack multi-camera person dataset p.3., p.5., p.7. </t>
   </si>
   <si>
-    <t>(Chavdarova, T. 2017)</t>
-  </si>
-  <si>
     <t>WILDTRACK dataset</t>
   </si>
   <si>
     <t>López-Cifuentes A.,Escudero-Viñolo M., 2018. Semantic Driven Multi-Camera Pedestrian Detection</t>
   </si>
   <si>
-    <t>(López-Cifuentes A. 2018)</t>
-  </si>
-  <si>
     <t>Y. C. Hou, M. Z. Baharuddin, S. Yussof and S. Dzulkifly, "Social Distancing Detection with Deep Learning Model," 2020</t>
   </si>
   <si>
-    <t>(Y. C. Hou, 2020)</t>
-  </si>
-  <si>
     <t>Existing systems</t>
+  </si>
+  <si>
+    <t>REDMON J., FARHADI A. "YOLOv3: An Incremental Improvement"</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>Deep learning architectures for object detection</t>
+  </si>
+  <si>
+    <t>Lin, T., Maire, M., Belongie, S., Bourdev, L., Girshick, R., Hays, J., Perona, P., Ramanan, D., Zitnick, C. and Dollar, P., 2021. Microsoft COCO: Common Objects in Context. [online] Arxiv.org. Available at: &lt;https://arxiv.org/pdf/1405.0312.pdf&gt; [Accessed 11 February 2021].</t>
+  </si>
+  <si>
+    <t>(Lin et al., 2021)</t>
+  </si>
+  <si>
+    <t>Pre-trained models (With COCO dataset)</t>
+  </si>
+  <si>
+    <t>(Y. C. Hou et al., 2020)</t>
+  </si>
+  <si>
+    <t>(López-Cifuentes A. et al., 2018)</t>
+  </si>
+  <si>
+    <t>(Coifman et al., 1998)</t>
+  </si>
+  <si>
+    <t>(Redmon et al.. 2018)</t>
+  </si>
+  <si>
+    <t>(Chavdarova et al. 2017)</t>
+  </si>
+  <si>
+    <t>Redmon, J., 2021. YOLO: Real-Time Object Detection. [online] Pjreddie.com. Available at: &lt;https://pjreddie.com/darknet/yolo/&gt; [Accessed 11 February 2021].</t>
+  </si>
+  <si>
+    <t>(Redmon, 2021)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -139,11 +172,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C281B7-8BDC-4908-A351-99DAA93660BA}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +522,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -519,7 +553,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -530,61 +564,104 @@
     </row>
     <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
       </c>
       <c r="D8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>22</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
result section update 18/03
</commit_message>
<xml_diff>
--- a/report/references.xlsx
+++ b/report/references.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\year3\IN3007-IndividualProject\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E2D8E8-D701-4D76-B2F2-794695BC6004}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A565B4-44C1-4AB7-9CF1-3DD5D06F44AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64E3EF4A-D857-422D-A798-7481F9C38A08}"/>
+    <workbookView xWindow="31680" yWindow="1410" windowWidth="21600" windowHeight="11385" xr2:uid="{64E3EF4A-D857-422D-A798-7481F9C38A08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>reference</t>
   </si>
@@ -131,6 +131,18 @@
   </si>
   <si>
     <t>(Redmon, 2021)</t>
+  </si>
+  <si>
+    <t>Docs.opencv.org. 2021. OpenCV: Basic concepts of the homography explained with code. [online] Available at: &lt;https://docs.opencv.org/master/d9/dab/tutorial_homography.html&gt; [Accessed 15 March 2021].</t>
+  </si>
+  <si>
+    <t>(OpenCV: Basic concepts of the homography explained with code, 2021)</t>
+  </si>
+  <si>
+    <t>results</t>
+  </si>
+  <si>
+    <t>Detecting Social Distancing by  bounding box</t>
   </si>
 </sst>
 </file>
@@ -492,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C281B7-8BDC-4908-A351-99DAA93660BA}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,6 +672,20 @@
         <v>24</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>